<commit_message>
Remove rockets with COPVs that are too big
Now the input handler checks if the rocket's COPV OD (plus a margin) is bigger than the tank OD. If it is, it removes the rocket from the possible rockets dataframe.
</commit_message>
<xml_diff>
--- a/data/inputs/rocket_defining_inputs.xlsx
+++ b/data/inputs/rocket_defining_inputs.xlsx
@@ -1,42 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27726"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\htfil\OneDrive\Documents\GitHub\PSPL_Rocket_4_Sizing\data\inputs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E86D3179-DA4E-47DB-8526-65FFCF56FEAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Continuous Inputs"/>
-    <sheet r:id="rId2" sheetId="2" name="Propellant Combinations"/>
-    <sheet r:id="rId3" sheetId="3" name="Tank Walls"/>
-    <sheet r:id="rId4" sheetId="4" name="COPVs"/>
+    <sheet name="Continuous Inputs" sheetId="1" r:id="rId1"/>
+    <sheet name="Propellant Combinations" sheetId="2" r:id="rId2"/>
+    <sheet name="Tank Walls" sheetId="3" r:id="rId3"/>
+    <sheet name="COPVs" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
   <si>
     <t>COPV name</t>
   </si>
   <si>
-    <t>COPV volume (in^3)</t>
-  </si>
-  <si>
-    <t>COPV pressure (psi)</t>
-  </si>
-  <si>
-    <t>COPV mass (lbm)</t>
-  </si>
-  <si>
-    <t>COPV length (in)</t>
-  </si>
-  <si>
-    <t>COPV diameter (in)</t>
-  </si>
-  <si>
     <t>COPV 1</t>
   </si>
   <si>
@@ -104,13 +95,28 @@
   </si>
   <si>
     <t>Step</t>
+  </si>
+  <si>
+    <t>Length (in)</t>
+  </si>
+  <si>
+    <t>Mass (lbm)</t>
+  </si>
+  <si>
+    <t>Pressure (psi)</t>
+  </si>
+  <si>
+    <t>Volume (liters)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="#,##0.000"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -160,50 +166,56 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+  <cellXfs count="13">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -214,10 +226,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -255,71 +267,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -347,7 +359,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -370,11 +382,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -383,13 +395,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -399,7 +411,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -408,7 +420,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -417,7 +429,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -425,10 +437,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -493,67 +505,66 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" style="11" width="6.147857142857143" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="6" width="20.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="9" width="20.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="5" width="14.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="6.109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.44140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
-      <c r="A1" s="10"/>
+    <row r="1" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="8"/>
       <c r="B1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>25</v>
+        <v>19</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>20</v>
       </c>
       <c r="D1" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row r="2" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" s="4">
+        <v>21</v>
+      </c>
+      <c r="B2" s="3">
         <v>100</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="3">
         <v>4</v>
       </c>
-      <c r="D2" s="3"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    </row>
+    <row r="3" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B3" s="4">
+        <v>22</v>
+      </c>
+      <c r="B3" s="3">
         <v>500</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="3">
         <v>5</v>
       </c>
-      <c r="D3" s="3"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    </row>
+    <row r="4" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B4" s="4">
-        <v>50</v>
-      </c>
-      <c r="C4" s="8">
-        <v>0.2</v>
-      </c>
-      <c r="D4" s="3"/>
+        <v>23</v>
+      </c>
+      <c r="B4" s="3">
+        <v>100</v>
+      </c>
+      <c r="C4" s="6">
+        <v>0.5</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -561,82 +572,84 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" style="5" width="21.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="5" width="15.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="6" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="9" width="14.005" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="9" width="13.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.88671875" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
+    <row r="1" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="B2" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="C2" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="D2" s="3">
+        <v>2</v>
+      </c>
+      <c r="E2" s="3">
+        <v>3</v>
+      </c>
+      <c r="F2" s="6">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
-      <c r="A2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" s="4">
-        <v>2</v>
-      </c>
-      <c r="E2" s="4">
-        <v>4</v>
-      </c>
-      <c r="F2" s="8">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
-      <c r="A3" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D3" s="4">
-        <v>2</v>
-      </c>
-      <c r="E3" s="8">
+      <c r="D3" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="E3" s="6">
         <v>3.5</v>
       </c>
-      <c r="F3" s="8">
-        <v>0.25</v>
+      <c r="F3" s="6">
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>
@@ -645,53 +658,135 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" style="5" width="37.14785714285715" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="9" width="16.005" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="37.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
+    <row r="1" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
-      <c r="A2" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="8">
+        <v>4</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="10">
         <v>6.625</v>
       </c>
-      <c r="C2" s="8">
-        <v>0.134</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
-      <c r="A3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="4">
+      <c r="C2" s="10">
+        <v>0.13400000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="8">
+      <c r="B3" s="10">
+        <v>7</v>
+      </c>
+      <c r="C3" s="10">
         <v>0.125</v>
       </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B15" s="11"/>
+      <c r="C15" s="11"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B16" s="11"/>
+      <c r="C16" s="11"/>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B18" s="11"/>
+      <c r="C18" s="11"/>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B20" s="11"/>
+      <c r="C20" s="11"/>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B21" s="11"/>
+      <c r="C21" s="11"/>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B22" s="11"/>
+      <c r="C22" s="11"/>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B23" s="11"/>
+      <c r="C23" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -699,82 +794,83 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" style="5" width="11.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="6" width="19.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="6" width="19.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="6" width="21.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="6" width="20.005" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="6" width="17.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="19.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.44140625" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row r="1" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="B2" s="12">
+        <v>10</v>
+      </c>
+      <c r="C2" s="12">
+        <v>5000</v>
+      </c>
+      <c r="D2" s="12">
+        <v>40</v>
+      </c>
+      <c r="E2" s="12">
+        <v>20</v>
+      </c>
+      <c r="F2" s="12">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
-      <c r="A2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="4">
-        <v>500</v>
-      </c>
-      <c r="C2" s="4">
-        <v>5000</v>
-      </c>
-      <c r="D2" s="4">
-        <v>40</v>
-      </c>
-      <c r="E2" s="4">
+      <c r="B3" s="12">
         <v>20</v>
       </c>
-      <c r="F2" s="4">
-        <v>6</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
-      <c r="A3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="4">
-        <v>700</v>
-      </c>
-      <c r="C3" s="4">
+      <c r="C3" s="12">
         <v>4000</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="12">
         <v>60</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="12">
         <v>30</v>
       </c>
-      <c r="F3" s="4">
-        <v>7</v>
+      <c r="F3" s="12">
+        <v>6.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Moved fluids test back to tests
</commit_message>
<xml_diff>
--- a/data/inputs/rocket_defining_inputs.xlsx
+++ b/data/inputs/rocket_defining_inputs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\School\Desktop\PSPL_Rocket_4_Sizing\data\inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7ab8326e43f711ef/Documents/GitHub/PSPL_Rocket_4_Sizing/data/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CE16149-0C16-418F-A83A-4CBB69E50DC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{8CE16149-0C16-418F-A83A-4CBB69E50DC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{27092EF7-7A98-4762-A17B-F2913B32093F}"/>
   <bookViews>
-    <workbookView xWindow="12673" yWindow="33" windowWidth="19200" windowHeight="11154" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Continuous Inputs" sheetId="1" r:id="rId1"/>
@@ -109,10 +109,10 @@
     <t>Methane</t>
   </si>
   <si>
-    <t>n-Dodecane</t>
-  </si>
-  <si>
     <t>Oxygen</t>
+  </si>
+  <si>
+    <t>Jet-A</t>
   </si>
 </sst>
 </file>
@@ -533,15 +533,15 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="6.1171875" style="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.5859375" style="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.41015625" style="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.29296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.08984375" style="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.54296875" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.36328125" style="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="14"/>
       <c r="B1" s="6" t="s">
         <v>21</v>
@@ -551,7 +551,7 @@
       </c>
       <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>23</v>
       </c>
@@ -562,7 +562,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>24</v>
       </c>
@@ -573,7 +573,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>25</v>
       </c>
@@ -597,20 +597,20 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5859375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.29296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.1171875" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.08984375" style="12" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14" style="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.87890625" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.90625" style="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -630,12 +630,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C2" t="s">
         <v>27</v>
@@ -650,15 +650,15 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>19</v>
       </c>
       <c r="B3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" t="s">
         <v>29</v>
-      </c>
-      <c r="C3" t="s">
-        <v>28</v>
       </c>
       <c r="D3" s="8">
         <v>2.5</v>
@@ -670,12 +670,12 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C4" t="s">
         <v>26</v>
@@ -704,14 +704,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="37.1171875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.7265625" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -722,7 +722,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -733,7 +733,7 @@
         <v>0.13400000000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -744,83 +744,83 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
     </row>
-    <row r="5" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
     </row>
-    <row r="6" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
     </row>
-    <row r="7" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
     </row>
-    <row r="8" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
     </row>
-    <row r="9" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
     </row>
-    <row r="10" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
     </row>
-    <row r="11" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
     </row>
-    <row r="12" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
     </row>
-    <row r="13" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
     </row>
-    <row r="14" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
     </row>
-    <row r="15" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
     </row>
-    <row r="16" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
     </row>
-    <row r="17" spans="2:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="17" spans="2:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
     </row>
-    <row r="18" spans="2:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="18" spans="2:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
     </row>
-    <row r="19" spans="2:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="19" spans="2:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
     </row>
-    <row r="20" spans="2:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="20" spans="2:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
     </row>
-    <row r="21" spans="2:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="21" spans="2:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
     </row>
-    <row r="22" spans="2:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="22" spans="2:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
     </row>
-    <row r="23" spans="2:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="23" spans="2:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
     </row>
@@ -838,16 +838,16 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="19.703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.29296875" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="19.7265625" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.26953125" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.41015625" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.36328125" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -867,7 +867,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -887,7 +887,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>7</v>
       </c>

</xml_diff>

<commit_message>
propulsion test script cms
</commit_message>
<xml_diff>
--- a/data/inputs/rocket_defining_inputs.xlsx
+++ b/data/inputs/rocket_defining_inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\School\Desktop\PSPL_Rocket_4_Sizing\data\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90E3CDA3-27D7-44E1-85A1-FF727E1E94F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{822BFE9A-EE50-460A-8F3B-76B93ADB85FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6480" yWindow="4180" windowWidth="19200" windowHeight="11180" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3300" yWindow="3300" windowWidth="19200" windowHeight="11180" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Continuous Inputs" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
   <si>
     <t>COPV name</t>
   </si>
@@ -64,12 +64,6 @@
     <t>Propellant combination</t>
   </si>
   <si>
-    <t>Oxidizer CEA</t>
-  </si>
-  <si>
-    <t>Fuel CEA</t>
-  </si>
-  <si>
     <t>O:F start (mass)</t>
   </si>
   <si>
@@ -82,22 +76,10 @@
     <t>Methalox</t>
   </si>
   <si>
-    <t>O2(L)</t>
-  </si>
-  <si>
-    <t>CH4(L)</t>
-  </si>
-  <si>
     <t>Kerolox</t>
   </si>
   <si>
-    <t>Jet-A(L)</t>
-  </si>
-  <si>
     <t>Ethalox</t>
-  </si>
-  <si>
-    <t>C2H5OH(L)</t>
   </si>
   <si>
     <t>Chamber pressure (psi)</t>
@@ -547,16 +529,16 @@
     <row r="1" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A1" s="11"/>
       <c r="B1" s="5" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D1" s="1"/>
     </row>
     <row r="2" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A2" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B2" s="7">
         <v>100</v>
@@ -567,7 +549,7 @@
     </row>
     <row r="3" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A3" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B3" s="7">
         <v>500</v>
@@ -578,7 +560,7 @@
     </row>
     <row r="4" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A4" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B4" s="7">
         <v>100</v>
@@ -597,10 +579,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -608,113 +590,88 @@
     <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.5859375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="17" customWidth="1"/>
-    <col min="6" max="6" width="14.1171875" style="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14" style="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.87890625" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.1171875" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14" style="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.87890625" style="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="6" t="s">
+    </row>
+    <row r="2" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A2" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="B2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="7">
+        <v>2</v>
+      </c>
+      <c r="E2" s="7">
+        <v>3</v>
+      </c>
+      <c r="F2" s="8">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A2" t="s">
+      <c r="B3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="E3" s="8">
+        <v>3.5</v>
+      </c>
+      <c r="F3" s="8">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A4" t="s">
         <v>18</v>
       </c>
-      <c r="B2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" s="7">
+      <c r="B4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="7">
+        <v>1</v>
+      </c>
+      <c r="E4" s="8">
         <v>2</v>
       </c>
-      <c r="G2" s="7">
-        <v>3</v>
-      </c>
-      <c r="H2" s="8">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F3" s="7">
-        <v>2.5</v>
-      </c>
-      <c r="G3" s="8">
-        <v>3.5</v>
-      </c>
-      <c r="H3" s="8">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F4" s="7">
-        <v>1</v>
-      </c>
-      <c r="G4" s="8">
-        <v>2</v>
-      </c>
-      <c r="H4" s="8">
+      <c r="F4" s="8">
         <v>0.5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
remove MR from main, utils
</commit_message>
<xml_diff>
--- a/data/inputs/rocket_defining_inputs.xlsx
+++ b/data/inputs/rocket_defining_inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\School\Desktop\PSPL_Rocket_4_Sizing\data\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{822BFE9A-EE50-460A-8F3B-76B93ADB85FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBAF8139-2595-4529-80F0-B17F8749EFF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3300" yWindow="3300" windowWidth="19200" windowHeight="11180" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38290" yWindow="12960" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Continuous Inputs" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
   <si>
     <t>COPV name</t>
   </si>
@@ -113,6 +113,9 @@
   </si>
   <si>
     <t>oxygen</t>
+  </si>
+  <si>
+    <t>Exit pressure (psi)</t>
   </si>
 </sst>
 </file>
@@ -514,29 +517,35 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="1" width="6.1171875" style="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.5859375" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.41015625" style="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.29296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.5859375" style="9" customWidth="1"/>
+    <col min="4" max="4" width="20.41015625" style="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.29296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A1" s="11"/>
       <c r="B1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="1"/>
-    </row>
-    <row r="2" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="E1" s="1"/>
+    </row>
+    <row r="2" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A2" s="1" t="s">
         <v>21</v>
       </c>
@@ -544,10 +553,13 @@
         <v>100</v>
       </c>
       <c r="C2" s="7">
+        <v>7</v>
+      </c>
+      <c r="D2" s="7">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A3" s="1" t="s">
         <v>22</v>
       </c>
@@ -555,10 +567,13 @@
         <v>500</v>
       </c>
       <c r="C3" s="7">
+        <v>13</v>
+      </c>
+      <c r="D3" s="7">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A4" s="1" t="s">
         <v>23</v>
       </c>
@@ -566,6 +581,9 @@
         <v>100</v>
       </c>
       <c r="C4" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="D4" s="8">
         <v>0.5</v>
       </c>
     </row>
@@ -581,8 +599,8 @@
   </sheetPr>
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>

</xml_diff>

<commit_message>
O/F with film cooling (part 2)
Improved outputs and changed O/F name in main and inputs sheet so it's clear that it's the core O/F
</commit_message>
<xml_diff>
--- a/data/inputs/rocket_defining_inputs.xlsx
+++ b/data/inputs/rocket_defining_inputs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\School\Desktop\PSPL_Rocket_4_Sizing\data\inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7ab8326e43f711ef/Documents/GitHub/PSPL_Rocket_4_Sizing/data/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44C58A26-4FDD-41EC-876B-984E027933FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{44C58A26-4FDD-41EC-876B-984E027933FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{15F11DA4-E2AF-42A9-AA86-7EF14C38BC22}"/>
   <bookViews>
-    <workbookView xWindow="2073" yWindow="4000" windowWidth="19200" windowHeight="11180" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Continuous Inputs" sheetId="1" r:id="rId1"/>
@@ -65,15 +65,6 @@
     <t>Fuel</t>
   </si>
   <si>
-    <t>O:F start (mass)</t>
-  </si>
-  <si>
-    <t>O:F stop (mass)</t>
-  </si>
-  <si>
-    <t>O:F step (mass)</t>
-  </si>
-  <si>
     <t>Methalox</t>
   </si>
   <si>
@@ -108,6 +99,15 @@
   </si>
   <si>
     <t>Height (ft)</t>
+  </si>
+  <si>
+    <t>Core O:F start (mass)</t>
+  </si>
+  <si>
+    <t>Core O:F stop (mass)</t>
+  </si>
+  <si>
+    <t>Core O:F step (mass)</t>
   </si>
 </sst>
 </file>
@@ -514,32 +514,34 @@
   </sheetPr>
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="6.1171875" style="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="20.5859375" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.41015625" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.29296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.08984375" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="20.54296875" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.36328125" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="9"/>
       <c r="B1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="1"/>
+    </row>
+    <row r="2" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E1" s="1"/>
-    </row>
-    <row r="2" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="B2" s="6">
         <v>200</v>
@@ -551,9 +553,9 @@
         <v>5.18</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B3" s="6">
         <v>200</v>
@@ -565,9 +567,9 @@
         <v>5.18</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B4" s="6">
         <v>100</v>
@@ -591,19 +593,21 @@
   </sheetPr>
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5859375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.54296875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.1171875" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.87890625" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.6328125" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.36328125" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.26953125" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -614,24 +618,24 @@
         <v>12</v>
       </c>
       <c r="D1" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="B2" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="C2" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" t="s">
-        <v>18</v>
       </c>
       <c r="D2" s="6">
         <v>2.7</v>
@@ -643,12 +647,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D3" s="7"/>
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
     </row>
-    <row r="4" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D4" s="7"/>
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
@@ -669,14 +673,14 @@
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="37.1171875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.7265625" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -687,7 +691,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -698,87 +702,87 @@
         <v>0.13400000000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
     </row>
-    <row r="4" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
     </row>
-    <row r="5" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
     </row>
-    <row r="6" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
     </row>
-    <row r="7" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
     </row>
-    <row r="8" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
     </row>
-    <row r="9" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
     </row>
-    <row r="10" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
     </row>
-    <row r="11" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
     </row>
-    <row r="12" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
     </row>
-    <row r="13" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
     </row>
-    <row r="14" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
     </row>
-    <row r="15" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
     </row>
-    <row r="16" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
     </row>
-    <row r="17" spans="2:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="17" spans="2:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
     </row>
-    <row r="18" spans="2:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="18" spans="2:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
     </row>
-    <row r="19" spans="2:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="19" spans="2:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
     </row>
-    <row r="20" spans="2:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="20" spans="2:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
     </row>
-    <row r="21" spans="2:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="21" spans="2:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
     </row>
-    <row r="22" spans="2:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="22" spans="2:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
     </row>
-    <row r="23" spans="2:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="23" spans="2:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
     </row>
@@ -796,16 +800,16 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="19.703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.29296875" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="19.7265625" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.26953125" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.41015625" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.36328125" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -825,7 +829,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -845,7 +849,7 @@
         <v>5.9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -861,32 +865,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4745E527-C9D9-49DB-AE90-F780F12EF05C}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="16.234375" customWidth="1"/>
+    <col min="2" max="2" width="16.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="11"/>
       <c r="B1" s="11" t="s">
         <v>3</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.5">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="11" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.5">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="11" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change COPV od margin to limits section
</commit_message>
<xml_diff>
--- a/data/inputs/rocket_defining_inputs.xlsx
+++ b/data/inputs/rocket_defining_inputs.xlsx
@@ -114,7 +114,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.000"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -126,12 +126,6 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -169,7 +163,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -181,7 +175,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -192,8 +186,11 @@
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -201,19 +198,13 @@
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -524,22 +515,22 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="15" width="6.005" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="4" width="6.005" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="13" width="20.576428571428572" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="13" width="20.576428571428572" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="13" width="20.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="4" width="14.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="9" width="14.290714285714287" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="14"/>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="11" t="s">
         <v>25</v>
       </c>
       <c r="E1" s="1"/>
@@ -548,13 +539,13 @@
       <c r="A2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="11">
+      <c r="B2" s="12">
         <v>200</v>
       </c>
-      <c r="C2" s="11">
+      <c r="C2" s="12">
         <v>11</v>
       </c>
-      <c r="D2" s="11">
+      <c r="D2" s="12">
         <v>5.18</v>
       </c>
       <c r="E2" s="7"/>
@@ -563,13 +554,13 @@
       <c r="A3" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="11">
+      <c r="B3" s="12">
         <v>200</v>
       </c>
-      <c r="C3" s="11">
+      <c r="C3" s="12">
         <v>11</v>
       </c>
-      <c r="D3" s="11">
+      <c r="D3" s="12">
         <v>5.18</v>
       </c>
       <c r="E3" s="7"/>
@@ -578,13 +569,13 @@
       <c r="A4" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="11">
+      <c r="B4" s="12">
         <v>100</v>
       </c>
-      <c r="C4" s="11">
+      <c r="C4" s="12">
         <v>1</v>
       </c>
-      <c r="D4" s="11">
+      <c r="D4" s="12">
         <v>1</v>
       </c>
       <c r="E4" s="7"/>
@@ -605,9 +596,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="4" width="21.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="4" width="17.005" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="9" width="21.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="9" width="17.005" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="13" width="18.719285714285714" customWidth="1" bestFit="1"/>
     <col min="5" max="5" style="13" width="18.290714285714284" customWidth="1" bestFit="1"/>
     <col min="6" max="6" style="13" width="18.290714285714284" customWidth="1" bestFit="1"/>
@@ -623,13 +614,13 @@
       <c r="C1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="11" t="s">
         <v>19</v>
       </c>
     </row>
@@ -643,13 +634,13 @@
       <c r="C2" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="11">
+      <c r="D2" s="12">
         <v>2.7</v>
       </c>
-      <c r="E2" s="11">
+      <c r="E2" s="12">
         <v>2.7</v>
       </c>
-      <c r="F2" s="11">
+      <c r="F2" s="12">
         <v>1</v>
       </c>
     </row>
@@ -657,17 +648,17 @@
       <c r="A3" s="7"/>
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="7"/>
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -685,9 +676,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="4" width="37.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="9" width="16.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="9" width="16.005" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="9" width="37.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="10" width="16.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="10" width="16.005" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -833,12 +824,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="4" width="11.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="9" width="19.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="9" width="19.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="9" width="21.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="9" width="20.005" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="9" width="17.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="9" width="11.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="10" width="19.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="10" width="19.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="10" width="21.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="10" width="20.005" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="10" width="17.290714285714284" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">

</xml_diff>

<commit_message>
holy fuck we r cookin
</commit_message>
<xml_diff>
--- a/data/inputs/rocket_defining_inputs.xlsx
+++ b/data/inputs/rocket_defining_inputs.xlsx
@@ -1,25 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27928"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7ab8326e43f711ef/Documents/GitHub/PSPL_Rocket_4_Sizing/data/inputs/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="11_43C237E33E762F1388A0889AAFBE2A7C1B3494E9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Continuous Inputs" sheetId="1" r:id="rId1"/>
-    <sheet name="Propellant Combinations" sheetId="2" r:id="rId2"/>
-    <sheet name="Tank Walls" sheetId="3" r:id="rId3"/>
-    <sheet name="COPVs" sheetId="4" r:id="rId4"/>
-    <sheet name="Limits" sheetId="5" r:id="rId5"/>
+    <sheet r:id="rId1" sheetId="1" name="Continuous Inputs"/>
+    <sheet r:id="rId2" sheetId="2" name="Propellant Combinations"/>
+    <sheet r:id="rId3" sheetId="3" name="Tank Walls"/>
+    <sheet r:id="rId4" sheetId="4" name="COPVs"/>
+    <sheet r:id="rId5" sheetId="5" name="Limits"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -116,7 +110,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.000"/>
   </numFmts>
@@ -169,56 +163,59 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="15">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="4" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" builtinId="0" name="Normal"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -229,10 +226,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -270,71 +267,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Times New Roman" script="Arab"/>
+        <a:font typeface="Times New Roman" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="MoolBoran" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Times New Roman" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Arial" script="Arab"/>
+        <a:font typeface="Arial" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="DaunPenh" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Arial" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -362,7 +359,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -385,11 +382,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -398,13 +395,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -414,7 +411,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -423,7 +420,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -432,7 +429,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -440,10 +437,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
+              <a:rot rev="0" lon="0" lat="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
+            <a:lightRig dir="t" rig="threePt">
+              <a:rot rev="1200000" lon="0" lat="0"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -508,78 +505,80 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
-    </sheetView>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="20.54296875" style="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.26953125" style="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="4" width="6.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="13" width="20.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="13" width="20.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="13" width="20.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="9" width="14.290714285714287" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="12"/>
-      <c r="B1" s="9" t="s">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+      <c r="A1" s="14"/>
+      <c r="B1" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="11" t="s">
         <v>25</v>
       </c>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="10">
+      <c r="B2" s="12">
         <v>200</v>
       </c>
-      <c r="C2" s="10">
+      <c r="C2" s="12">
         <v>11</v>
       </c>
-      <c r="D2" s="10">
+      <c r="D2" s="12">
         <v>5.18</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E2" s="7"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="10">
+      <c r="B3" s="12">
         <v>300</v>
       </c>
-      <c r="C3" s="10">
+      <c r="C3" s="12">
         <v>11</v>
       </c>
-      <c r="D3" s="10">
+      <c r="D3" s="12">
         <v>5.18</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E3" s="7"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="10">
-        <v>0.1</v>
-      </c>
-      <c r="C4" s="10">
+      <c r="B4" s="12">
         <v>1</v>
       </c>
-      <c r="D4" s="10">
+      <c r="C4" s="12">
         <v>1</v>
       </c>
+      <c r="D4" s="12">
+        <v>1</v>
+      </c>
+      <c r="E4" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -587,7 +586,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -595,16 +594,17 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.7265625" style="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="18.26953125" style="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="9" width="21.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="9" width="17.005" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="13" width="18.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="13" width="18.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="13" width="18.290714285714284" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -614,45 +614,51 @@
       <c r="C1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="11" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
+      <c r="A2" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="10">
+      <c r="D2" s="12">
         <v>2.7</v>
       </c>
-      <c r="E2" s="10">
+      <c r="E2" s="12">
         <v>2.7</v>
       </c>
-      <c r="F2" s="10">
+      <c r="F2" s="12">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
+      <c r="A3" s="7"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
       <c r="D3" s="3"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-    </row>
-    <row r="4" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
+      <c r="A4" s="7"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
       <c r="D4" s="3"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -660,7 +666,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -668,14 +674,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.7265625" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="9" width="37.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="10" width="16.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="10" width="16.005" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -686,100 +692,121 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
+      <c r="A2" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="7">
+      <c r="B2" s="8">
         <v>6.625</v>
       </c>
-      <c r="C2" s="7">
-        <v>0.13400000000000001</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-    </row>
-    <row r="4" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-    </row>
-    <row r="5" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-    </row>
-    <row r="6" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-    </row>
-    <row r="7" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-    </row>
-    <row r="8" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-    </row>
-    <row r="9" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-    </row>
-    <row r="10" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-    </row>
-    <row r="11" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-    </row>
-    <row r="12" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-    </row>
-    <row r="13" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-    </row>
-    <row r="14" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-    </row>
-    <row r="15" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-    </row>
-    <row r="16" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-    </row>
-    <row r="17" spans="2:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-    </row>
-    <row r="18" spans="2:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-    </row>
-    <row r="19" spans="2:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-    </row>
-    <row r="20" spans="2:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-    </row>
-    <row r="21" spans="2:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
-    </row>
-    <row r="22" spans="2:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
-    </row>
-    <row r="23" spans="2:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
+      <c r="C2" s="8">
+        <v>0.134</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
+      <c r="A3" s="7"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
+      <c r="A4" s="7"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
+      <c r="A5" s="7"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
+      <c r="A6" s="7"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
+      <c r="A7" s="7"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
+      <c r="A8" s="7"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
+      <c r="A9" s="7"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
+      <c r="A10" s="7"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
+      <c r="A11" s="7"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
+      <c r="A12" s="7"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
+      <c r="A13" s="7"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
+      <c r="A14" s="7"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
+      <c r="A15" s="7"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
+      <c r="A16" s="7"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
+      <c r="A17" s="7"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
+      <c r="A18" s="7"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
+      <c r="A19" s="7"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
+      <c r="A20" s="7"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
+      <c r="A21" s="7"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
+      <c r="A22" s="7"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
+      <c r="A23" s="7"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -787,7 +814,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -795,16 +822,17 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="19.7265625" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.26953125" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.26953125" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="9" width="11.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="10" width="19.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="10" width="19.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="10" width="21.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="10" width="20.005" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="10" width="17.290714285714284" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -824,32 +852,33 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+      <c r="A2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="7">
-        <v>9.0128900000000005</v>
-      </c>
-      <c r="C2" s="7">
+      <c r="B2" s="8">
+        <v>9.01289</v>
+      </c>
+      <c r="C2" s="8">
         <v>4945</v>
       </c>
-      <c r="D2" s="7">
+      <c r="D2" s="8">
         <v>12.5</v>
       </c>
-      <c r="E2" s="7">
+      <c r="E2" s="8">
         <v>31.9</v>
       </c>
-      <c r="F2" s="7">
+      <c r="F2" s="8">
         <v>5.9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+      <c r="A3" s="7"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -857,24 +886,22 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.54296875" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.26953125" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="5" width="16.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -883,7 +910,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -894,7 +921,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
delete the big fucking file
</commit_message>
<xml_diff>
--- a/data/inputs/rocket_defining_inputs.xlsx
+++ b/data/inputs/rocket_defining_inputs.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="49">
   <si>
     <t>Thrust (lbf)</t>
   </si>
@@ -137,13 +137,13 @@
     <t>Core O:F step (mass)</t>
   </si>
   <si>
-    <t>Methalox</t>
+    <t>Ethalox</t>
   </si>
   <si>
     <t>oxygen</t>
   </si>
   <si>
-    <t>methane</t>
+    <t>ethanol</t>
   </si>
   <si>
     <t>Chamber pressure (psi)</t>
@@ -163,6 +163,9 @@
   <si>
     <t>Step</t>
   </si>
+  <si>
+    <t>s</t>
+  </si>
 </sst>
 </file>
 
@@ -171,7 +174,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -189,6 +192,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -240,8 +249,8 @@
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -643,175 +652,177 @@
       </c>
       <c r="E4" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="6"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
       <c r="E5" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="6"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
       <c r="E6" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="6"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
       <c r="E7" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="6"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
       <c r="E8" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="6"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
       <c r="E9" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="6"/>
-      <c r="B10" s="5"/>
+      <c r="B10" s="5" t="s">
+        <v>48</v>
+      </c>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
       <c r="E10" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="6"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
       <c r="E11" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="6"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
       <c r="E12" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="6"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
       <c r="E13" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="6"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="6"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
       <c r="E15" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
       <c r="A16" s="6"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
       <c r="E16" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
       <c r="A17" s="6"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
       <c r="E17" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
       <c r="A18" s="6"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
       <c r="E18" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
       <c r="A19" s="6"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
       <c r="E19" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
       <c r="A20" s="6"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
       <c r="E20" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
       <c r="A21" s="6"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
       <c r="E21" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
       <c r="A22" s="6"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
       <c r="E22" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
       <c r="A23" s="6"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
       <c r="E23" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
       <c r="A24" s="6"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
       <c r="E24" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
       <c r="A25" s="6"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
       <c r="E25" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">
       <c r="A26" s="6"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
       <c r="E26" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5">
       <c r="A27" s="6"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
       <c r="E27" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="19.5">
       <c r="A28" s="6"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
       <c r="E28" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="19.5">
       <c r="A29" s="6"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
@@ -7670,10 +7681,10 @@
         <v>41</v>
       </c>
       <c r="D2" s="5">
-        <v>2.5</v>
+        <v>1.5</v>
       </c>
       <c r="E2" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F2" s="5">
         <v>0.1</v>

</xml_diff>

<commit_message>
Added pump pressure rise
</commit_message>
<xml_diff>
--- a/data/inputs/rocket_defining_inputs.xlsx
+++ b/data/inputs/rocket_defining_inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7ab8326e43f711ef/Documents/GitHub/PSPL_Rocket_4_Sizing/data/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="11_833B7F5E8EAB49EC0F7FCFFE2BC93964CA0BE476" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{74DC4734-5CB2-4E43-B0EA-821A68391488}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="11_833B7F5E8EAB49EC0F7FCFFE2BC93964CA0BE476" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{209E45CE-7DF2-4762-9220-72B6FD947F0F}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Continuous Inputs" sheetId="1" r:id="rId1"/>
@@ -546,8 +546,8 @@
   </sheetPr>
   <dimension ref="A1:E1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -27195,7 +27195,7 @@
   </sheetPr>
   <dimension ref="A1:H1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>

</xml_diff>

<commit_message>
Why were COPV parameters changed
</commit_message>
<xml_diff>
--- a/data/inputs/rocket_defining_inputs.xlsx
+++ b/data/inputs/rocket_defining_inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7ab8326e43f711ef/Documents/GitHub/PSPL_Rocket_4_Sizing/data/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="11_833B7F5E8EAB49EC0F7FCFFE2BC93964CA0BE476" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{209E45CE-7DF2-4762-9220-72B6FD947F0F}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="11_833B7F5E8EAB49EC0F7FCFFE2BC93964CA0BE476" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F702C3D8-0C90-4525-9D9F-0422FBE9E991}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Continuous Inputs" sheetId="1" r:id="rId1"/>
@@ -546,7 +546,7 @@
   </sheetPr>
   <dimension ref="A1:E1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -19644,7 +19644,9 @@
   </sheetPr>
   <dimension ref="A1:F938"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -19683,16 +19685,16 @@
         <v>18.100000000000001</v>
       </c>
       <c r="C2" s="14">
-        <v>4931.28</v>
+        <v>4935</v>
       </c>
       <c r="D2" s="14">
-        <v>15.83</v>
+        <v>22.5</v>
       </c>
       <c r="E2" s="14">
-        <v>8.11</v>
+        <v>31.3</v>
       </c>
       <c r="F2" s="14">
-        <v>8.11</v>
+        <v>8.1</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">

</xml_diff>